<commit_message>
Update : Small fix and meta updates
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/EternalAwakeningMeta.xlsx
+++ b/Excel_and_CSV/EternalAwakeningMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F767B6-1DB5-4963-B0AF-4780C93D07FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FC1EEA-9CE7-4DD2-BAD3-293747629D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
+    <workbookView xWindow="30" yWindow="0" windowWidth="20370" windowHeight="10620" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="188">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Forbidden Darkmage</t>
   </si>
   <si>
-    <t>Karyl Rune</t>
-  </si>
-  <si>
     <t>Princess Knight</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Dragon-Devouring Dread</t>
   </si>
   <si>
-    <t>Aggro Dragon</t>
-  </si>
-  <si>
     <t>Wyrmfire Engineer</t>
   </si>
   <si>
@@ -216,24 +210,12 @@
     <t>Nephthys, Goddess of Amenta</t>
   </si>
   <si>
-    <t>Bone Fanatic</t>
-  </si>
-  <si>
     <t>Fieran, Havensent Wind God</t>
   </si>
   <si>
-    <t>Reanimate Gremory Shadow</t>
-  </si>
-  <si>
     <t>Fatal Order</t>
   </si>
   <si>
-    <t>Invincible Monster Trio</t>
-  </si>
-  <si>
-    <t>Gremory Shadow</t>
-  </si>
-  <si>
     <t>Sarcophagus Wraith</t>
   </si>
   <si>
@@ -291,9 +273,6 @@
     <t>Ra, Radiance Incarnate</t>
   </si>
   <si>
-    <t>Rally Haven</t>
-  </si>
-  <si>
     <t>Goddess of the West Wind</t>
   </si>
   <si>
@@ -450,15 +429,9 @@
     <t>70OYc</t>
   </si>
   <si>
-    <t>745Mi</t>
-  </si>
-  <si>
     <t>6-UTy</t>
   </si>
   <si>
-    <t>74ChS</t>
-  </si>
-  <si>
     <t>gXuCg</t>
   </si>
   <si>
@@ -531,9 +504,6 @@
     <t>79A3y</t>
   </si>
   <si>
-    <t>Burial-Rite Rally (BRR) Shadow</t>
-  </si>
-  <si>
     <t>Vincent Spell Rune</t>
   </si>
   <si>
@@ -547,13 +517,85 @@
   </si>
   <si>
     <t>Evolution OTK Portal</t>
+  </si>
+  <si>
+    <t>Control Karyl Rune</t>
+  </si>
+  <si>
+    <t>0. Lhynkal, The Fool</t>
+  </si>
+  <si>
+    <t>6_djI</t>
+  </si>
+  <si>
+    <t>Turbo Karyl Rune</t>
+  </si>
+  <si>
+    <t>Control Ra Haven</t>
+  </si>
+  <si>
+    <t>Summit Haven</t>
+  </si>
+  <si>
+    <t>Vergewalker Magician</t>
+  </si>
+  <si>
+    <t>6xkhy</t>
+  </si>
+  <si>
+    <t>78lSg</t>
+  </si>
+  <si>
+    <t>Summit Temple</t>
+  </si>
+  <si>
+    <t>6Qzmg</t>
+  </si>
+  <si>
+    <t>Rally Shadow</t>
+  </si>
+  <si>
+    <t>Gremory (Reanimate) Shadow</t>
+  </si>
+  <si>
+    <t>Gremory (Standard) Shadow</t>
+  </si>
+  <si>
+    <t>Gremory (Rally) Shadow</t>
+  </si>
+  <si>
+    <t>77ygg</t>
+  </si>
+  <si>
+    <t>Undead Parade</t>
+  </si>
+  <si>
+    <t>Face Dragon</t>
+  </si>
+  <si>
+    <t>Whale Dragon</t>
+  </si>
+  <si>
+    <t>Eternal Whale</t>
+  </si>
+  <si>
+    <t>6_zhi</t>
+  </si>
+  <si>
+    <t>Slaughtering Dragonewt</t>
+  </si>
+  <si>
+    <t>6_zhY</t>
+  </si>
+  <si>
+    <t>West Wind(Rally) Haven</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -584,6 +626,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -633,7 +681,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -651,6 +699,10 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -967,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,19 +1048,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1022,13 +1074,13 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>9</v>
@@ -1048,13 +1100,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -1074,13 +1126,13 @@
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>9</v>
@@ -1100,19 +1152,19 @@
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1126,13 +1178,13 @@
         <v>19</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>9</v>
@@ -1152,13 +1204,13 @@
         <v>22</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -1169,7 +1221,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
@@ -1178,13 +1230,13 @@
         <v>29</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1204,19 +1256,19 @@
         <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1227,16 +1279,16 @@
         <v>25</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>9</v>
@@ -1256,13 +1308,13 @@
         <v>33</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>
@@ -1282,13 +1334,13 @@
         <v>33</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>9</v>
@@ -1299,7 +1351,7 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>32</v>
@@ -1308,13 +1360,13 @@
         <v>35</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -1325,7 +1377,7 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>32</v>
@@ -1334,13 +1386,13 @@
         <v>35</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -1357,16 +1409,16 @@
         <v>32</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>127</v>
+        <v>171</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
@@ -1377,7 +1429,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>32</v>
@@ -1386,13 +1438,13 @@
         <v>37</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>128</v>
+        <v>166</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
@@ -1403,22 +1455,22 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>41</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>130</v>
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>9</v>
@@ -1429,22 +1481,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>134</v>
+      <c r="D18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>123</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
@@ -1455,22 +1507,22 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
@@ -1481,22 +1533,22 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
@@ -1507,256 +1559,256 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>58</v>
-      </c>
       <c r="F22" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>146</v>
+        <v>99</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>182</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>9</v>
+      <c r="H24" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H25" s="2" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H26" s="2" t="s">
-        <v>9</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>68</v>
+        <v>178</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H28" s="4" t="s">
+      <c r="F28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H28" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>73</v>
+      <c r="A29" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>76</v>
+        <v>177</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>9</v>
@@ -1766,75 +1818,75 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>79</v>
+      <c r="A31" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H32" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>9</v>
@@ -1845,74 +1897,74 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H35" s="2" t="s">
-        <v>9</v>
+        <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>94</v>
+      <c r="A36" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>164</v>
+        <v>76</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>9</v>
@@ -1923,22 +1975,22 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>95</v>
+        <v>76</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>9</v>
@@ -1949,27 +2001,183 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="2" t="s">
+      <c r="D39" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature : Add Coloring for lineup and misc addons
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/EternalAwakeningMeta.xlsx
+++ b/Excel_and_CSV/EternalAwakeningMeta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FC1EEA-9CE7-4DD2-BAD3-293747629D6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDB9B20-AE2B-4476-8348-AD27C04D64F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="0" windowWidth="20370" windowHeight="10620" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="204">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Lionel, Woodland Shadow</t>
   </si>
   <si>
-    <t>Chipper Skipper</t>
-  </si>
-  <si>
     <t>Loxis, Homestead Pioneer</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>Fatal Order</t>
   </si>
   <si>
-    <t>Sarcophagus Wraith</t>
-  </si>
-  <si>
     <t>Volteo Blood</t>
   </si>
   <si>
@@ -342,9 +336,6 @@
     <t>6-qSC</t>
   </si>
   <si>
-    <t>6-qS2</t>
-  </si>
-  <si>
     <t>72h1S</t>
   </si>
   <si>
@@ -378,9 +369,6 @@
     <t>6_djc</t>
   </si>
   <si>
-    <t>Vincent Amulet Rune</t>
-  </si>
-  <si>
     <t>73RsS</t>
   </si>
   <si>
@@ -444,9 +432,6 @@
     <t>6xRA6</t>
   </si>
   <si>
-    <t>6yXzC</t>
-  </si>
-  <si>
     <t>74b5o</t>
   </si>
   <si>
@@ -504,21 +489,9 @@
     <t>79A3y</t>
   </si>
   <si>
-    <t>Vincent Spell Rune</t>
-  </si>
-  <si>
-    <t>Impalement Arts</t>
-  </si>
-  <si>
-    <t>779PQ</t>
-  </si>
-  <si>
     <t>Evolution Sword</t>
   </si>
   <si>
-    <t>Evolution OTK Portal</t>
-  </si>
-  <si>
     <t>Control Karyl Rune</t>
   </si>
   <si>
@@ -558,12 +531,6 @@
     <t>Gremory (Reanimate) Shadow</t>
   </si>
   <si>
-    <t>Gremory (Standard) Shadow</t>
-  </si>
-  <si>
-    <t>Gremory (Rally) Shadow</t>
-  </si>
-  <si>
     <t>77ygg</t>
   </si>
   <si>
@@ -588,7 +555,88 @@
     <t>6_zhY</t>
   </si>
   <si>
-    <t>West Wind(Rally) Haven</t>
+    <t>Gremory Shadow</t>
+  </si>
+  <si>
+    <t>74ChS</t>
+  </si>
+  <si>
+    <t>Invincible Monster Trio</t>
+  </si>
+  <si>
+    <t>Niyon, Mystic Musician</t>
+  </si>
+  <si>
+    <t>780qI</t>
+  </si>
+  <si>
+    <t>Evolution Shadow</t>
+  </si>
+  <si>
+    <t>Vyrn, Li'l Red Dragon</t>
+  </si>
+  <si>
+    <t>764JY</t>
+  </si>
+  <si>
+    <t>Heal Blood</t>
+  </si>
+  <si>
+    <t>Craps Devil</t>
+  </si>
+  <si>
+    <t>74WDI</t>
+  </si>
+  <si>
+    <t>Mallet Monkey</t>
+  </si>
+  <si>
+    <t>6t7Hs</t>
+  </si>
+  <si>
+    <t>Vincent (Runie) Rune</t>
+  </si>
+  <si>
+    <t>West Wind (Rally) Haven</t>
+  </si>
+  <si>
+    <t>Evolution Portal</t>
+  </si>
+  <si>
+    <t>Vincent (Vehicle) Rune</t>
+  </si>
+  <si>
+    <t>Fairy Flowering</t>
+  </si>
+  <si>
+    <t>72fJw</t>
+  </si>
+  <si>
+    <t>Happy Pig Rune</t>
+  </si>
+  <si>
+    <t>Sweetspell Sorcerer</t>
+  </si>
+  <si>
+    <t>6_Yqy</t>
+  </si>
+  <si>
+    <t>Maiser, Neighborhood Hero</t>
+  </si>
+  <si>
+    <t>73RsI</t>
+  </si>
+  <si>
+    <t>Aggro Rune</t>
+  </si>
+  <si>
+    <t>Rivaylian Bandit</t>
+  </si>
+  <si>
+    <t>72BI2</t>
+  </si>
+  <si>
+    <t>Maiser Rune</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
-  <dimension ref="A1:H44"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,19 +1096,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1074,19 +1122,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>9</v>
+        <v>188</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1100,13 +1148,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -1117,100 +1165,100 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>9</v>
+      <c r="G4" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>106</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -1221,22 +1269,22 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1247,48 +1295,48 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="H9" s="4" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>9</v>
@@ -1299,22 +1347,22 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>
@@ -1325,48 +1373,48 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>99</v>
+      <c r="E13" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -1376,23 +1424,23 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>159</v>
+      <c r="A14" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>161</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -1403,22 +1451,22 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>36</v>
+        <v>189</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>120</v>
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>113</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>171</v>
+        <v>34</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
@@ -1428,23 +1476,23 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>164</v>
+      <c r="A16" s="4" t="s">
+        <v>192</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>119</v>
+        <v>34</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>166</v>
+        <v>34</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
@@ -1454,23 +1502,23 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>167</v>
+      <c r="A17" s="4" t="s">
+        <v>195</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>119</v>
+        <v>196</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>197</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>121</v>
+        <v>198</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>9</v>
@@ -1480,23 +1528,23 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>40</v>
+      <c r="A18" s="4" t="s">
+        <v>200</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>43</v>
+        <v>199</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>123</v>
+        <v>202</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
@@ -1506,23 +1554,23 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>50</v>
+      <c r="A19" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>126</v>
+        <v>198</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>127</v>
+        <v>201</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
@@ -1533,22 +1581,22 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>44</v>
+        <v>158</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
@@ -1559,22 +1607,22 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>129</v>
+      <c r="D21" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>119</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>9</v>
@@ -1585,22 +1633,22 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>181</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>99</v>
+        <v>51</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>9</v>
@@ -1611,22 +1659,22 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>182</v>
+        <v>43</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>183</v>
+        <v>44</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>184</v>
+        <v>120</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>186</v>
+        <v>45</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
@@ -1636,257 +1684,257 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>54</v>
+      <c r="A24" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>137</v>
+        <v>47</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>58</v>
+        <v>170</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>133</v>
+        <v>8</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>97</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>9</v>
+      <c r="F27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>176</v>
+        <v>57</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>62</v>
+        <v>169</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>168</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>9</v>
+        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>70</v>
+        <v>176</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>9</v>
@@ -1896,75 +1944,75 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>73</v>
+      <c r="A34" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>9</v>
@@ -1975,22 +2023,22 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>9</v>
@@ -2001,183 +2049,287 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="F39" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D38" s="2" t="s">
+      <c r="B41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F38" s="2" t="s">
+      <c r="G46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="G38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B39" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D39" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="B40" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>174</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="G47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" s="2" t="s">
+      <c r="D48" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F43" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="2" t="s">
+      <c r="F48" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Last Patch before JCG website Revamp
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/EternalAwakeningMeta.xlsx
+++ b/Excel_and_CSV/EternalAwakeningMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDB9B20-AE2B-4476-8348-AD27C04D64F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB30F5E-C8FF-42A4-A440-4B24A21E991C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="207">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Accelerate Forest</t>
   </si>
   <si>
-    <t>Lionel, Woodland Shadow</t>
-  </si>
-  <si>
     <t>Loxis, Homestead Pioneer</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>Wrath Blood</t>
   </si>
   <si>
-    <t>Aragavy the Berserker</t>
-  </si>
-  <si>
     <t>Darhold, Abyssal Contract</t>
   </si>
   <si>
@@ -333,9 +327,6 @@
     <t>6-mIQ</t>
   </si>
   <si>
-    <t>6-qSC</t>
-  </si>
-  <si>
     <t>72h1S</t>
   </si>
   <si>
@@ -441,9 +432,6 @@
     <t>6ywNi</t>
   </si>
   <si>
-    <t>6v8go</t>
-  </si>
-  <si>
     <t>70myy</t>
   </si>
   <si>
@@ -637,6 +625,27 @@
   </si>
   <si>
     <t>Maiser Rune</t>
+  </si>
+  <si>
+    <t>Aggro Blood</t>
+  </si>
+  <si>
+    <t>Silverbolt Hunter</t>
+  </si>
+  <si>
+    <t>70feC</t>
+  </si>
+  <si>
+    <t>Permafrost Behemoth</t>
+  </si>
+  <si>
+    <t>6v8h6</t>
+  </si>
+  <si>
+    <t>6-lZs</t>
+  </si>
+  <si>
+    <t>Deepwood Wolf</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1076,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,19 +1105,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1122,19 +1131,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1148,13 +1157,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -1165,28 +1174,28 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1200,13 +1209,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
@@ -1223,16 +1232,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>102</v>
+        <v>205</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
@@ -1243,22 +1252,22 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -1269,22 +1278,22 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1295,48 +1304,48 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="H9" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>9</v>
@@ -1347,22 +1356,22 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>
@@ -1373,22 +1382,22 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>9</v>
@@ -1399,22 +1408,22 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -1425,22 +1434,22 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -1451,22 +1460,22 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="F15" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
@@ -1477,22 +1486,22 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
@@ -1503,22 +1512,22 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>199</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>9</v>
@@ -1529,22 +1538,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>198</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
@@ -1555,22 +1564,22 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
@@ -1581,22 +1590,22 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
@@ -1607,22 +1616,22 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>42</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>9</v>
@@ -1633,22 +1642,22 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>9</v>
@@ -1659,22 +1668,22 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
@@ -1685,22 +1694,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>9</v>
@@ -1711,22 +1720,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>9</v>
@@ -1737,22 +1746,22 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>171</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>175</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>9</v>
@@ -1763,100 +1772,100 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="H27" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>9</v>
@@ -1867,22 +1876,22 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>9</v>
@@ -1893,48 +1902,48 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>9</v>
@@ -1945,22 +1954,22 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>9</v>
@@ -1971,22 +1980,22 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>9</v>
@@ -1997,22 +2006,22 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>9</v>
@@ -2023,22 +2032,22 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>9</v>
@@ -2049,22 +2058,22 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>9</v>
@@ -2074,75 +2083,75 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="D40" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="4" t="s">
+      <c r="F40" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H40" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>9</v>
@@ -2153,74 +2162,74 @@
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>190</v>
+        <v>80</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="B43" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="F43" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" s="7" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>164</v>
-      </c>
       <c r="D44" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E44" s="8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G44" s="7" t="s">
         <v>9</v>
@@ -2229,24 +2238,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>79</v>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>79</v>
+        <v>161</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>160</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>9</v>
@@ -2256,49 +2265,49 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="A46" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="D47" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>151</v>
+      <c r="F47" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>9</v>
@@ -2309,27 +2318,53 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>191</v>
+        <v>87</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="H48" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
card update for mini expansion
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/EternalAwakeningMeta.xlsx
+++ b/Excel_and_CSV/EternalAwakeningMeta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB30F5E-C8FF-42A4-A440-4B24A21E991C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA82B39-FD59-47F2-B9B7-143F3456DDB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="210">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Amelia, the Silverflash</t>
   </si>
   <si>
-    <t>Kagemitsu, Matchless Blade</t>
-  </si>
-  <si>
     <t>Seofon, Star Sword Sovereign</t>
   </si>
   <si>
@@ -342,9 +339,6 @@
     <t>Stroke of Conviction</t>
   </si>
   <si>
-    <t>6td0o</t>
-  </si>
-  <si>
     <t>76tay</t>
   </si>
   <si>
@@ -646,6 +640,21 @@
   </si>
   <si>
     <t>Deepwood Wolf</t>
+  </si>
+  <si>
+    <t>Eahta, God of the Blade</t>
+  </si>
+  <si>
+    <t>76tao</t>
+  </si>
+  <si>
+    <t>Aggro Ravening Blood</t>
+  </si>
+  <si>
+    <t>6yrV2</t>
+  </si>
+  <si>
+    <t>Vampiric Bloodbinder</t>
   </si>
 </sst>
 </file>
@@ -1076,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,19 +1114,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1131,19 +1140,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1157,13 +1166,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -1183,19 +1192,19 @@
         <v>17</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1209,13 +1218,13 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
@@ -1232,16 +1241,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
@@ -1261,13 +1270,13 @@
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -1277,23 +1286,23 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>150</v>
+      <c r="A8" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1303,75 +1312,75 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
-        <v>24</v>
+      <c r="A9" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E9" s="4" t="s">
+      <c r="D10" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="F10" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="H10" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C11" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E10" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>110</v>
+      <c r="F11" t="s">
+        <v>102</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>
@@ -1382,23 +1391,23 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>110</v>
-      </c>
       <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
@@ -1407,23 +1416,23 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>34</v>
+      <c r="A13" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>158</v>
+      <c r="D13" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -1434,22 +1443,22 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>151</v>
+        <v>33</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -1460,48 +1469,48 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="F16" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
@@ -1512,22 +1521,22 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>193</v>
+        <v>109</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>194</v>
+        <v>32</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>195</v>
+        <v>109</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>9</v>
@@ -1538,22 +1547,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
@@ -1564,48 +1573,48 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="B20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>114</v>
+      <c r="F20" s="4" t="s">
+        <v>193</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
@@ -1616,22 +1625,22 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>152</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>116</v>
+        <v>29</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>9</v>
@@ -1642,22 +1651,22 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>120</v>
+      <c r="D22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>114</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>9</v>
@@ -1668,19 +1677,19 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>117</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>118</v>
@@ -1694,22 +1703,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>9</v>
@@ -1720,22 +1729,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>166</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>95</v>
+        <v>46</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>9</v>
@@ -1746,152 +1755,152 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="F27" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="G27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="F28" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G28" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="H28" s="2" t="s">
-        <v>130</v>
+      <c r="H28" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>162</v>
+        <v>55</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>165</v>
+        <v>56</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>164</v>
+        <v>123</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="D30" s="2" t="s">
-        <v>129</v>
+        <v>162</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>9</v>
@@ -1902,178 +1911,178 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>178</v>
+        <v>59</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>175</v>
+        <v>54</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>176</v>
+        <v>128</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>173</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H33" s="2" t="s">
-        <v>9</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>61</v>
+      <c r="A34" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="D37" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="F37" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>180</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>181</v>
+        <v>201</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>182</v>
+        <v>202</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>96</v>
+        <v>133</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>9</v>
@@ -2084,287 +2093,339 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>200</v>
+        <v>68</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>8</v>
+        <v>69</v>
       </c>
       <c r="D39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>75</v>
+        <v>198</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D41" s="2" t="s">
+      <c r="D42" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H42" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>186</v>
+        <v>74</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" s="7" t="s">
+      <c r="F45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="E44" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F44" s="7" t="s">
+      <c r="E47" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F47" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H45" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H46" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="G47" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C49" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D49" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="F49" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F47" s="4" t="s">
+      <c r="G50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F48" s="2" t="s">
+      <c r="E51" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H49" s="2" t="s">
+      <c r="G51" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feature : trend finder
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/EternalAwakeningMeta.xlsx
+++ b/Excel_and_CSV/EternalAwakeningMeta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA82B39-FD59-47F2-B9B7-143F3456DDB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673B203-2C74-43D3-9CFB-C9B8F70ED9F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="214">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Terrorformer</t>
   </si>
   <si>
-    <t>Evolve Forest</t>
-  </si>
-  <si>
     <t>Phantasmal Fairy Dragon</t>
   </si>
   <si>
@@ -177,9 +174,6 @@
     <t>Dragon-Devouring Dread</t>
   </si>
   <si>
-    <t>Wyrmfire Engineer</t>
-  </si>
-  <si>
     <t>Aggro Shadow</t>
   </si>
   <si>
@@ -390,9 +384,6 @@
     <t>6-Ntw</t>
   </si>
   <si>
-    <t>73iyC</t>
-  </si>
-  <si>
     <t>745MY</t>
   </si>
   <si>
@@ -510,9 +501,6 @@
     <t>Rally Shadow</t>
   </si>
   <si>
-    <t>Gremory (Reanimate) Shadow</t>
-  </si>
-  <si>
     <t>77ygg</t>
   </si>
   <si>
@@ -576,18 +564,12 @@
     <t>6t7Hs</t>
   </si>
   <si>
-    <t>Vincent (Runie) Rune</t>
-  </si>
-  <si>
     <t>West Wind (Rally) Haven</t>
   </si>
   <si>
     <t>Evolution Portal</t>
   </si>
   <si>
-    <t>Vincent (Vehicle) Rune</t>
-  </si>
-  <si>
     <t>Fairy Flowering</t>
   </si>
   <si>
@@ -630,12 +612,6 @@
     <t>70feC</t>
   </si>
   <si>
-    <t>Permafrost Behemoth</t>
-  </si>
-  <si>
-    <t>6v8h6</t>
-  </si>
-  <si>
     <t>6-lZs</t>
   </si>
   <si>
@@ -648,13 +624,49 @@
     <t>76tao</t>
   </si>
   <si>
-    <t>Aggro Ravening Blood</t>
-  </si>
-  <si>
-    <t>6yrV2</t>
-  </si>
-  <si>
-    <t>Vampiric Bloodbinder</t>
+    <t>70M62</t>
+  </si>
+  <si>
+    <t>Deathbringer</t>
+  </si>
+  <si>
+    <t>Deathbringer Shadow</t>
+  </si>
+  <si>
+    <t>Evolution Forest</t>
+  </si>
+  <si>
+    <t>Vincent Rune</t>
+  </si>
+  <si>
+    <t>Razia, Vengeful Cannonlancer</t>
+  </si>
+  <si>
+    <t>77bzY</t>
+  </si>
+  <si>
+    <t>Reggie, Peerless Artisan</t>
+  </si>
+  <si>
+    <t>73qGy</t>
+  </si>
+  <si>
+    <t>Scrappy Werewolf</t>
+  </si>
+  <si>
+    <t>74Tn2</t>
+  </si>
+  <si>
+    <t>Corruption Blood</t>
+  </si>
+  <si>
+    <t>Aggro Float Portal</t>
+  </si>
+  <si>
+    <t>75H2I</t>
+  </si>
+  <si>
+    <t>Capsule Homunculus</t>
   </si>
 </sst>
 </file>
@@ -1087,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,19 +1126,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1140,19 +1152,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1166,13 +1178,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -1183,48 +1195,48 @@
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>202</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
@@ -1235,22 +1247,22 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
@@ -1261,22 +1273,22 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="F7" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -1296,13 +1308,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1313,22 +1325,22 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -1339,48 +1351,48 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>26</v>
-      </c>
       <c r="H10" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>
@@ -1391,22 +1403,22 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>9</v>
@@ -1417,22 +1429,22 @@
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>108</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -1443,22 +1455,22 @@
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -1469,22 +1481,22 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
@@ -1494,23 +1506,23 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>183</v>
+      <c r="A16" s="4" t="s">
+        <v>203</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
@@ -1521,22 +1533,22 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F17" s="4" t="s">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>9</v>
@@ -1547,22 +1559,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="F18" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
@@ -1573,22 +1585,22 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
@@ -1598,23 +1610,23 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>197</v>
+      <c r="A20" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>193</v>
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>193</v>
+        <v>35</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
@@ -1625,21 +1637,21 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>152</v>
+        <v>36</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F21" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>112</v>
       </c>
       <c r="G21" s="2" t="s">
@@ -1651,22 +1663,22 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>114</v>
+      <c r="C22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>116</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>9</v>
@@ -1677,22 +1689,22 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
@@ -1703,22 +1715,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>9</v>
@@ -1729,22 +1741,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>119</v>
+        <v>205</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>120</v>
+        <v>206</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>9</v>
@@ -1755,152 +1767,152 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="F26" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>128</v>
+      <c r="H28" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>157</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>160</v>
+        <v>201</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>163</v>
+        <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>58</v>
+        <v>200</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>125</v>
+        <v>199</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>128</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>161</v>
+        <v>201</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>54</v>
+        <v>200</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>9</v>
@@ -1911,178 +1923,178 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>59</v>
+        <v>172</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>126</v>
+        <v>173</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>54</v>
+        <v>169</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>128</v>
+        <v>170</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>176</v>
-      </c>
       <c r="D33" s="2" t="s">
-        <v>177</v>
+        <v>125</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>173</v>
+        <v>52</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>174</v>
+        <v>125</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>172</v>
+        <v>9</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>171</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>170</v>
+      <c r="A34" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H34" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>62</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H36" s="4" t="s">
+      <c r="G36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H36" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>63</v>
+      <c r="A37" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E37" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H37" s="4" t="s">
+      <c r="E37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H37" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>9</v>
@@ -2093,22 +2105,22 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>68</v>
+        <v>192</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>69</v>
+        <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>134</v>
+        <v>92</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>69</v>
+        <v>193</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>134</v>
+        <v>194</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>9</v>
@@ -2119,22 +2131,22 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>9</v>
@@ -2144,153 +2156,153 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>198</v>
+      <c r="A41" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>200</v>
+        <v>69</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>70</v>
+      <c r="A42" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G43" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H43" s="2" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>79</v>
+        <v>179</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H45" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H45" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>9</v>
@@ -2299,24 +2311,24 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>158</v>
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>158</v>
+        <v>135</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>159</v>
+        <v>135</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>9</v>
@@ -2326,49 +2338,49 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="G48" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H48" s="7" t="s">
+      <c r="A48" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
-        <v>82</v>
+      <c r="A49" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="E49" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F49" s="4" t="s">
-        <v>144</v>
+      <c r="F49" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>9</v>
@@ -2379,22 +2391,22 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>58</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>87</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>9</v>
@@ -2404,23 +2416,23 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>147</v>
+      <c r="A51" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
+        <v>213</v>
+      </c>
+      <c r="D51" t="s">
+        <v>212</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" t="s">
+        <v>92</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Feature : Convert SVO Format and misc update
</commit_message>
<xml_diff>
--- a/Excel_and_CSV/EternalAwakeningMeta.xlsx
+++ b/Excel_and_CSV/EternalAwakeningMeta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python_WS\Github_SV\Excel_and_CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6673B203-2C74-43D3-9CFB-C9B8F70ED9F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AB9AF1-2DF9-4957-8084-2CA186C758FA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7EC583D9-1A7C-40BB-9E54-3D901F246F53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="216">
   <si>
     <t>Archetype Name</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Forbidden Darkmage</t>
   </si>
   <si>
-    <t>Princess Knight</t>
-  </si>
-  <si>
     <t>Discard Dragon</t>
   </si>
   <si>
@@ -357,9 +354,6 @@
     <t>6t_Rc</t>
   </si>
   <si>
-    <t>6spli</t>
-  </si>
-  <si>
     <t>6yB-y</t>
   </si>
   <si>
@@ -543,12 +537,6 @@
     <t>Evolution Shadow</t>
   </si>
   <si>
-    <t>Vyrn, Li'l Red Dragon</t>
-  </si>
-  <si>
-    <t>764JY</t>
-  </si>
-  <si>
     <t>Heal Blood</t>
   </si>
   <si>
@@ -600,9 +588,6 @@
     <t>72BI2</t>
   </si>
   <si>
-    <t>Maiser Rune</t>
-  </si>
-  <si>
     <t>Aggro Blood</t>
   </si>
   <si>
@@ -667,6 +652,27 @@
   </si>
   <si>
     <t>Capsule Homunculus</t>
+  </si>
+  <si>
+    <t>Evolution Rune</t>
+  </si>
+  <si>
+    <t>Fif, Prodigious Sorcerer</t>
+  </si>
+  <si>
+    <t>77F_I</t>
+  </si>
+  <si>
+    <t>Combustion Demon</t>
+  </si>
+  <si>
+    <t>764Js</t>
+  </si>
+  <si>
+    <t>745Mi</t>
+  </si>
+  <si>
+    <t>Bone Fanatic</t>
   </si>
 </sst>
 </file>
@@ -1099,8 +1105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F11DFBF7-9F71-4179-B5F3-8C061A06A61C}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,19 +1132,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1152,19 +1158,19 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1178,13 +1184,13 @@
         <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>9</v>
@@ -1204,24 +1210,24 @@
         <v>16</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
@@ -1230,13 +1236,13 @@
         <v>13</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>9</v>
@@ -1253,16 +1259,16 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>9</v>
@@ -1282,13 +1288,13 @@
         <v>19</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -1308,13 +1314,13 @@
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -1325,22 +1331,22 @@
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -1360,19 +1366,19 @@
         <v>24</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1383,16 +1389,16 @@
         <v>22</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>101</v>
-      </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>
@@ -1412,13 +1418,13 @@
         <v>29</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>9</v>
@@ -1438,13 +1444,13 @@
         <v>29</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>9</v>
@@ -1464,13 +1470,13 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>9</v>
@@ -1481,7 +1487,7 @@
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>28</v>
@@ -1490,13 +1496,13 @@
         <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>9</v>
@@ -1507,7 +1513,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>28</v>
@@ -1516,13 +1522,13 @@
         <v>31</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>9</v>
@@ -1533,22 +1539,22 @@
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>9</v>
@@ -1559,22 +1565,22 @@
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>186</v>
+        <v>210</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>190</v>
+        <v>211</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>9</v>
@@ -1585,22 +1591,22 @@
     </row>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>186</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>187</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>9</v>
@@ -1611,7 +1617,7 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>28</v>
@@ -1620,13 +1626,13 @@
         <v>33</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>9</v>
@@ -1637,22 +1643,22 @@
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>39</v>
-      </c>
       <c r="F21" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>9</v>
@@ -1663,22 +1669,22 @@
     </row>
     <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>9</v>
@@ -1689,22 +1695,22 @@
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="F23" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>9</v>
@@ -1715,22 +1721,22 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>9</v>
@@ -1741,22 +1747,22 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>9</v>
@@ -1767,22 +1773,22 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="F26" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>165</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>9</v>
@@ -1793,100 +1799,100 @@
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="H27" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="F28" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>9</v>
@@ -1897,22 +1903,22 @@
     </row>
     <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>9</v>
@@ -1923,48 +1929,48 @@
     </row>
     <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>173</v>
+        <v>213</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>9</v>
@@ -1975,22 +1981,22 @@
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C34" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="D34" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>9</v>
@@ -2001,22 +2007,22 @@
     </row>
     <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D35" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="F35" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>9</v>
@@ -2027,22 +2033,22 @@
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>9</v>
@@ -2053,22 +2059,22 @@
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="D37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>9</v>
@@ -2079,22 +2085,22 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>9</v>
@@ -2105,22 +2111,22 @@
     </row>
     <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>9</v>
@@ -2131,22 +2137,22 @@
     </row>
     <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>9</v>
@@ -2157,48 +2163,48 @@
     </row>
     <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="F41" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="F42" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>9</v>
@@ -2209,48 +2215,48 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>79</v>
-      </c>
       <c r="F43" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="F44" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>9</v>
@@ -2261,22 +2267,22 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>9</v>
@@ -2287,22 +2293,22 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G46" s="7" t="s">
         <v>9</v>
@@ -2313,22 +2319,22 @@
     </row>
     <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>9</v>
@@ -2339,22 +2345,22 @@
     </row>
     <row r="48" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D48" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="F48" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>9</v>
@@ -2365,22 +2371,22 @@
     </row>
     <row r="49" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="F49" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>9</v>
@@ -2391,22 +2397,22 @@
     </row>
     <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="F50" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>9</v>
@@ -2417,22 +2423,22 @@
     </row>
     <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D51" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>8</v>
       </c>
       <c r="F51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>9</v>

</xml_diff>